<commit_message>
created new subtest and added other apis for validation
</commit_message>
<xml_diff>
--- a/rootFolder/subTest-1/ScenarioLayer-1/Main.rvl.xlsx
+++ b/rootFolder/subTest-1/ScenarioLayer-1/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="402" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="465" uniqueCount="115">
   <si>
     <t>Flow</t>
   </si>
@@ -307,6 +307,57 @@
   </si>
   <si>
     <t>responseBody.data[3]</t>
+  </si>
+  <si>
+    <t>SoftAssertNull</t>
+  </si>
+  <si>
+    <t>responseBody.data[]</t>
+  </si>
+  <si>
+    <t>responseBody.data[""]</t>
+  </si>
+  <si>
+    <t>responseBody.data["Hard disk size"]</t>
+  </si>
+  <si>
+    <t>And validate Hard disk size field present or not</t>
+  </si>
+  <si>
+    <t>Repository</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Map</t>
+  </si>
+  <si>
+    <t>Rows</t>
+  </si>
+  <si>
+    <t>demoMap</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>of Map</t>
+  </si>
+  <si>
+    <t>Loop</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Loop body</t>
+  </si>
+  <si>
+    <t>of Loop</t>
   </si>
 </sst>
 </file>
@@ -327,7 +378,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="199">
+  <borders count="213">
     <border>
       <left/>
       <right/>
@@ -533,11 +584,25 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -737,6 +802,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="196" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="197" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="198" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="199" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="200" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="201" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="202" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="203" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="204" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="205" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="206" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="207" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="208" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="209" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="210" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="211" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="212" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,7 +825,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection/>
@@ -791,539 +870,485 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
+      <c r="A2" s="212"/>
     </row>
     <row r="3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="24"/>
+      <c r="A3" s="211" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="25"/>
-      <c r="B4" s="26" t="s">
+      <c r="A4" s="210"/>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="209"/>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="208"/>
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="207" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="206"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="205" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="204" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="203"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="202" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C15" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D15" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E15" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="31" t="s">
+      <c r="F15" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="32"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="41"/>
-      <c r="B5" s="42" t="s">
+      <c r="H15" s="32"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="41"/>
+      <c r="B16" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C16" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D16" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E16" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="48"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="161"/>
-      <c r="B6" t="s">
+      <c r="F16" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="48"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="161"/>
+      <c r="B17" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E17" t="s">
         <v>13</v>
       </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="162"/>
-      <c r="B7" t="s">
+    <row r="18">
+      <c r="A18" s="162"/>
+      <c r="B18" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E18" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="163"/>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="164"/>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="165"/>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="89"/>
-      <c r="B11" s="90" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="91" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="92" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="93" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="94" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="95" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="96"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="169"/>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="166"/>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="105"/>
-      <c r="B14" s="106"/>
-      <c r="C14" s="107"/>
-      <c r="D14" s="108"/>
-      <c r="E14" s="109"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="111"/>
-      <c r="H14" s="112"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="113"/>
-      <c r="B15" s="114" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="115" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="116" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="117" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="118" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="119" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" s="120"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="167"/>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="121"/>
-      <c r="B17" s="122"/>
-      <c r="C17" s="123"/>
-      <c r="D17" s="124"/>
-      <c r="E17" s="125"/>
-      <c r="F17" s="126"/>
-      <c r="G17" s="127"/>
-      <c r="H17" s="128"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="129"/>
-      <c r="B18" s="130" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="131" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="132" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="133" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="134" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="135" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" s="136"/>
-    </row>
     <row r="19">
-      <c r="A19" s="170"/>
+      <c r="A19" s="163"/>
       <c r="B19" t="s">
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="G19" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="171"/>
+      <c r="A20" s="164"/>
       <c r="B20" t="s">
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="F20" t="s">
         <v>11</v>
       </c>
       <c r="G20" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="137"/>
-      <c r="B21" s="138"/>
-      <c r="C21" s="139"/>
-      <c r="D21" s="140"/>
-      <c r="E21" s="141"/>
-      <c r="F21" s="142"/>
-      <c r="G21" s="143"/>
-      <c r="H21" s="144"/>
+      <c r="A21" s="165"/>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="145"/>
-      <c r="B22" s="146" t="s">
+      <c r="A22" s="201" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="147" t="s">
+      <c r="C22" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="148" t="s">
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="169"/>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="166"/>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="105"/>
+      <c r="B25" s="106"/>
+      <c r="C25" s="107"/>
+      <c r="D25" s="108"/>
+      <c r="E25" s="109"/>
+      <c r="F25" s="110"/>
+      <c r="G25" s="111"/>
+      <c r="H25" s="112"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="113"/>
+      <c r="B26" s="114" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="115" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="149" t="s">
+      <c r="E26" s="117" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="150" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="151" t="s">
-        <v>57</v>
-      </c>
-      <c r="H22" s="152"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="173"/>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="153"/>
-      <c r="B24" s="154"/>
-      <c r="C24" s="155"/>
-      <c r="D24" s="156"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="158"/>
-      <c r="G24" s="159"/>
-      <c r="H24" s="160"/>
-    </row>
-    <row r="25">
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="177"/>
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" t="s">
-        <v>37</v>
-      </c>
-      <c r="G26" t="s">
-        <v>63</v>
-      </c>
+      <c r="F26" s="118" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="119" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="120"/>
     </row>
     <row r="27">
-      <c r="A27" s="178"/>
+      <c r="A27" s="167"/>
       <c r="B27" t="s">
         <v>12</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G27" t="s">
-        <v>24</v>
-      </c>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="121"/>
+      <c r="B28" s="122"/>
+      <c r="C28" s="123"/>
+      <c r="D28" s="124"/>
+      <c r="E28" s="125"/>
+      <c r="F28" s="126"/>
+      <c r="G28" s="127"/>
+      <c r="H28" s="128"/>
     </row>
     <row r="29">
-      <c r="B29" t="s">
+      <c r="A29" s="129"/>
+      <c r="B29" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="131" t="s">
         <v>33</v>
       </c>
-      <c r="D29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D29" s="132" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="133" t="s">
         <v>35</v>
       </c>
-      <c r="F29" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" t="s">
-        <v>64</v>
-      </c>
+      <c r="F29" s="134" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="135" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29" s="136"/>
     </row>
     <row r="30">
-      <c r="A30" s="181"/>
+      <c r="A30" s="170"/>
       <c r="B30" t="s">
         <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="F30" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G30" t="s">
-        <v>65</v>
-      </c>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="137"/>
+      <c r="B31" s="138"/>
+      <c r="C31" s="139"/>
+      <c r="D31" s="140"/>
+      <c r="E31" s="141"/>
+      <c r="F31" s="142"/>
+      <c r="G31" s="143"/>
+      <c r="H31" s="144"/>
     </row>
     <row r="32">
-      <c r="B32" t="s">
+      <c r="A32" s="145"/>
+      <c r="B32" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="147" t="s">
         <v>33</v>
       </c>
-      <c r="D32" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D32" s="148" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="149" t="s">
         <v>35</v>
       </c>
-      <c r="F32" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" t="s">
-        <v>85</v>
-      </c>
+      <c r="F32" s="150" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="151" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32" s="152"/>
     </row>
     <row r="33">
-      <c r="A33" s="184"/>
+      <c r="A33" s="173"/>
       <c r="B33" t="s">
         <v>12</v>
       </c>
       <c r="E33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="153"/>
+      <c r="B34" s="154"/>
+      <c r="C34" s="155"/>
+      <c r="D34" s="156"/>
+      <c r="E34" s="157"/>
+      <c r="F34" s="158"/>
+      <c r="G34" s="159"/>
+      <c r="H34" s="160"/>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="177"/>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
         <v>48</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F36" t="s">
         <v>37</v>
       </c>
-      <c r="G33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="185"/>
-      <c r="B34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" t="s">
-        <v>37</v>
-      </c>
-      <c r="G34" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" t="s">
-        <v>35</v>
-      </c>
-      <c r="F36" t="s">
-        <v>11</v>
-      </c>
       <c r="G36" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="187"/>
+      <c r="A37" s="178"/>
       <c r="B37" t="s">
         <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F37" t="s">
         <v>11</v>
       </c>
       <c r="G37" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39">
@@ -1334,7 +1359,7 @@
         <v>33</v>
       </c>
       <c r="D39" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="E39" t="s">
         <v>35</v>
@@ -1343,53 +1368,176 @@
         <v>11</v>
       </c>
       <c r="G39" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="198"/>
+      <c r="A40" s="181"/>
       <c r="B40" t="s">
         <v>12</v>
       </c>
       <c r="E40" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="F40" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="G40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="188"/>
+        <v>65</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="189"/>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="190"/>
+      <c r="A43" s="184"/>
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" t="s">
+        <v>48</v>
+      </c>
+      <c r="F43" t="s">
+        <v>37</v>
+      </c>
+      <c r="G43" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="191"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="192"/>
+      <c r="A44" s="185"/>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" t="s">
+        <v>49</v>
+      </c>
+      <c r="F44" t="s">
+        <v>37</v>
+      </c>
+      <c r="G44" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" s="193"/>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" t="s">
+        <v>34</v>
+      </c>
+      <c r="E46" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" s="194"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="195"/>
+      <c r="A47" s="187"/>
+      <c r="B47" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" t="s">
+        <v>36</v>
+      </c>
+      <c r="F47" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="196"/>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="197"/>
+      <c r="A50" s="200"/>
+      <c r="B50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" t="s">
+        <v>36</v>
+      </c>
+      <c r="F50" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="188"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="189"/>
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="190"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="191"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="192"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="193"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="194"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="195"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="196"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="197"/>
     </row>
   </sheetData>
   <tableParts/>

</xml_diff>

<commit_message>
new subtest and rest files are added for student management system
</commit_message>
<xml_diff>
--- a/rootFolder/subTest-1/ScenarioLayer-1/Main.rvl.xlsx
+++ b/rootFolder/subTest-1/ScenarioLayer-1/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="465" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="522" uniqueCount="121">
   <si>
     <t>Flow</t>
   </si>
@@ -358,6 +358,24 @@
   </si>
   <si>
     <t>of Loop</t>
+  </si>
+  <si>
+    <t>responseBody[0].name</t>
+  </si>
+  <si>
+    <t>SoftAssertGreater</t>
+  </si>
+  <si>
+    <t>n1</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>n2</t>
   </si>
 </sst>
 </file>
@@ -378,7 +396,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="213">
+  <borders count="220">
     <border>
       <left/>
       <right/>
@@ -598,11 +616,18 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="213">
+  <cellXfs count="220">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -816,6 +841,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="210" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="211" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="212" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="214" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="215" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="216" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="218" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="219" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,7 +857,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection/>
@@ -935,307 +967,314 @@
       <c r="A11" s="203"/>
     </row>
     <row r="12">
-      <c r="A12" s="202" t="s">
-        <v>109</v>
-      </c>
-      <c r="B12" t="s">
-        <v>114</v>
-      </c>
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
+      <c r="A13" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14">
-      <c r="A14" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" s="18" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26" t="s">
+      <c r="A15" s="41"/>
+      <c r="B15" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="32"/>
+      <c r="C15" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="G15" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="48"/>
     </row>
     <row r="16">
-      <c r="A16" s="41"/>
-      <c r="B16" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="46" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="48"/>
+      <c r="A16" s="161"/>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="161"/>
+      <c r="A17" s="162"/>
       <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="162"/>
+      <c r="A18" s="163"/>
       <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F18" t="s">
         <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="163"/>
+      <c r="A19" s="164"/>
       <c r="B19" t="s">
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s">
         <v>11</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="164"/>
+      <c r="A20" s="165"/>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G20" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="165"/>
+      <c r="A21" s="201" t="s">
+        <v>7</v>
+      </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="G21" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="H21" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="201" t="s">
-        <v>7</v>
-      </c>
+      <c r="A22" s="169"/>
       <c r="B22" t="s">
         <v>3</v>
       </c>
       <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="166"/>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="105"/>
+      <c r="B24" s="106"/>
+      <c r="C24" s="107"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="109"/>
+      <c r="F24" s="110"/>
+      <c r="G24" s="111"/>
+      <c r="H24" s="112"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="113"/>
+      <c r="B25" s="114" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="D22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D25" s="116" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="117" t="s">
         <v>35</v>
       </c>
-      <c r="F22" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" t="s">
-        <v>42</v>
-      </c>
-      <c r="H22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="169"/>
-      <c r="B23" t="s">
+      <c r="F25" s="118" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="119" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" s="120"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="167"/>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="121"/>
+      <c r="B27" s="122"/>
+      <c r="C27" s="123"/>
+      <c r="D27" s="124"/>
+      <c r="E27" s="125"/>
+      <c r="F27" s="126"/>
+      <c r="G27" s="127"/>
+      <c r="H27" s="128"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="129"/>
+      <c r="B28" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="166"/>
-      <c r="B24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="105"/>
-      <c r="B25" s="106"/>
-      <c r="C25" s="107"/>
-      <c r="D25" s="108"/>
-      <c r="E25" s="109"/>
-      <c r="F25" s="110"/>
-      <c r="G25" s="111"/>
-      <c r="H25" s="112"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="113"/>
-      <c r="B26" s="114" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="115" t="s">
+      <c r="C28" s="131" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="116" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" s="117" t="s">
+      <c r="D28" s="132" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="133" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="118" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="119" t="s">
-        <v>46</v>
-      </c>
-      <c r="H26" s="120"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="167"/>
-      <c r="B27" t="s">
+      <c r="F28" s="134" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="135" t="s">
+        <v>50</v>
+      </c>
+      <c r="H28" s="136"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="218"/>
+      <c r="B29" t="s">
         <v>12</v>
       </c>
-      <c r="E27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" t="s">
-        <v>37</v>
-      </c>
-      <c r="G27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="121"/>
-      <c r="B28" s="122"/>
-      <c r="C28" s="123"/>
-      <c r="D28" s="124"/>
-      <c r="E28" s="125"/>
-      <c r="F28" s="126"/>
-      <c r="G28" s="127"/>
-      <c r="H28" s="128"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="129"/>
-      <c r="B29" s="130" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="131" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="132" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="133" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" s="134" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" s="135" t="s">
-        <v>50</v>
-      </c>
-      <c r="H29" s="136"/>
+      <c r="E29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" t="s">
+        <v>107</v>
+      </c>
+      <c r="G29" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="170"/>
+      <c r="A30" s="219"/>
       <c r="B30" t="s">
         <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F30" t="s">
         <v>37</v>
@@ -1510,34 +1549,42 @@
       <c r="A51" s="188"/>
     </row>
     <row r="52">
-      <c r="A52" s="189"/>
+      <c r="A52" s="213" t="s">
+        <v>109</v>
+      </c>
       <c r="B52" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="189"/>
+      <c r="B53" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="190"/>
-    </row>
     <row r="54">
-      <c r="A54" s="191"/>
+      <c r="A54" s="190"/>
     </row>
     <row r="55">
-      <c r="A55" s="192"/>
+      <c r="A55" s="191"/>
     </row>
     <row r="56">
-      <c r="A56" s="193"/>
+      <c r="A56" s="192"/>
     </row>
     <row r="57">
-      <c r="A57" s="194"/>
+      <c r="A57" s="193"/>
     </row>
     <row r="58">
-      <c r="A58" s="195"/>
+      <c r="A58" s="194"/>
     </row>
     <row r="59">
-      <c r="A59" s="196"/>
+      <c r="A59" s="195"/>
     </row>
     <row r="60">
-      <c r="A60" s="197"/>
+      <c r="A60" s="196"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="197"/>
     </row>
   </sheetData>
   <tableParts/>

</xml_diff>